<commit_message>
AITATR3-122 RSV Personal Based On Rule
</commit_message>
<xml_diff>
--- a/Rule/InsuranceRateRule.xlsx
+++ b/Rule/InsuranceRateRule.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willis.wy\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeremy.andreas\git\NAP-CF4W-UF-Sept\Rule\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19815" windowHeight="7815" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19815" windowHeight="7815" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="AssetCategory" sheetId="1" r:id="rId1"/>
@@ -1622,8 +1622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2406,8 +2406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
AITATR3-150 Verify main rate based on rule
</commit_message>
<xml_diff>
--- a/Rule/InsuranceRateRule.xlsx
+++ b/Rule/InsuranceRateRule.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willis.wy\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeremy.andreas\git\NAP-CF4W-UF-11END\Rule\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19815" windowHeight="7815" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19815" windowHeight="7815" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AssetCategory" sheetId="1" r:id="rId1"/>
@@ -617,7 +617,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B20" sqref="A20:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -821,7 +821,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1092,8 +1092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1622,8 +1622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C23" sqref="A21:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2406,9 +2406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>

</xml_diff>

<commit_message>
Tambhan verify ddl NAP4 cust detail
</commit_message>
<xml_diff>
--- a/Rule/InsuranceRateRule.xlsx
+++ b/Rule/InsuranceRateRule.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeremy.andreas\git\NAP-CF4W-UF-11END\Rule\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeremy.andreas\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19815" windowHeight="7815" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="AssetCategory" sheetId="1" r:id="rId1"/>
@@ -1092,7 +1092,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+    <sheetView topLeftCell="C7" workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -1623,7 +1623,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C23" sqref="A21:C23"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2406,7 +2406,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -2683,7 +2685,7 @@
         <v>69</v>
       </c>
       <c r="J18" s="4">
-        <v>800000</v>
+        <v>1200000</v>
       </c>
       <c r="K18" s="4">
         <v>800000</v>
@@ -2788,7 +2790,7 @@
         <v>69</v>
       </c>
       <c r="J21" s="4">
-        <v>800000</v>
+        <v>1000000</v>
       </c>
       <c r="K21" s="4">
         <v>800000</v>

</xml_diff>